<commit_message>
update datasets, new datasets, some descriptive analysis by me
</commit_message>
<xml_diff>
--- a/Testzahlen.xlsx
+++ b/Testzahlen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Wissdaten\RKI_nCoV-Lage\3.Kommunikation\4.6.Laborergebnisse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6C7FA9-BCD4-410B-9567-117F412DABC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CBBF1A-140E-4DD6-8389-CF1CD104CB04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="14265" windowHeight="8100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0_Erläuterungen" sheetId="7" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="108">
   <si>
     <t>Das RKI erfasst wöchentlich die SARS-CoV-2-Testzahlen. Hierfür werden deutschlandweit Daten von Universitätskliniken, Forschungseinrichtungen sowie klinischen und ambulanten Laboren zusammengeführt. Die Erfassung basiert auf einer freiwilligen Mitteilung der Labore und erfolgt über eine webbasierte Plattform (VOXCO, RKI-Testlaborabfrage) oder in Zusammenarbeit mit der am RKI etablierten, laborbasierten SARS-CoV-2-Surveillance (eine Erweiterung der Antibiotika-Resistenz-Surveillance, ARS), dem Netzwerk für respiratorische Viren (RespVir) sowie der Abfrage eines labormedizinischen Berufsverbands. Die Erfassung liefert Hinweise zur aktuellen Situation in den Laboren, erlaubt aber keine detaillierten Auswertungen oder Vergleiche mit den gemeldeten Fallzahlen.</t>
   </si>
@@ -309,10 +309,13 @@
     <t>44/2021</t>
   </si>
   <si>
+    <t>45/2021</t>
+  </si>
+  <si>
     <t>Summe</t>
   </si>
   <si>
-    <t>Bis einschließlich KW34/2021</t>
+    <t>Bis einschließlich KW35/2021</t>
   </si>
   <si>
     <t>KW, für die die Angabe prognostisch erfolgt ist</t>
@@ -330,7 +333,7 @@
     <t>Reale Testkapazität zum Zeitpunkt der Abfrage</t>
   </si>
   <si>
-    <t>45/2021</t>
+    <t>46/2021</t>
   </si>
   <si>
     <t>Labore mit Rückstau</t>
@@ -457,7 +460,7 @@
   <cellStyles count="3">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="2" xr:uid="{996114FF-8DB1-4E86-B8D3-4C9995559A18}"/>
+    <cellStyle name="Standard 2" xfId="2" xr:uid="{382EAF50-33AD-404A-BB3C-B9BC4F55B996}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -768,7 +771,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD4B2E2-5059-42F6-8C08-9F7C24A464A8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F957158-0058-4CD4-BFFA-C68B159E4E65}">
   <dimension ref="A3:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -787,12 +790,12 @@
     </row>
     <row r="4" spans="1:1" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -820,6 +823,1871 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E91"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>69493</v>
+      </c>
+      <c r="C2">
+        <v>1722</v>
+      </c>
+      <c r="D2" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E2" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>129291</v>
+      </c>
+      <c r="C3">
+        <v>7502</v>
+      </c>
+      <c r="D3">
+        <v>5.8024147079069692</v>
+      </c>
+      <c r="E3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>374534</v>
+      </c>
+      <c r="C4">
+        <v>25886</v>
+      </c>
+      <c r="D4">
+        <v>6.9115220514025424</v>
+      </c>
+      <c r="E4">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>377599</v>
+      </c>
+      <c r="C5">
+        <v>33139</v>
+      </c>
+      <c r="D5">
+        <v>8.7762414625038723</v>
+      </c>
+      <c r="E5">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>417646</v>
+      </c>
+      <c r="C6">
+        <v>37649</v>
+      </c>
+      <c r="D6">
+        <v>9.0145721496195339</v>
+      </c>
+      <c r="E6">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>383694</v>
+      </c>
+      <c r="C7">
+        <v>30727</v>
+      </c>
+      <c r="D7">
+        <v>8.0082044545914197</v>
+      </c>
+      <c r="E7">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>339983</v>
+      </c>
+      <c r="C8">
+        <v>22724</v>
+      </c>
+      <c r="D8">
+        <v>6.6838636049449534</v>
+      </c>
+      <c r="E8">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>363659</v>
+      </c>
+      <c r="C9">
+        <v>18127</v>
+      </c>
+      <c r="D9">
+        <v>4.984614707734444</v>
+      </c>
+      <c r="E9">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>327799</v>
+      </c>
+      <c r="C10">
+        <v>12600</v>
+      </c>
+      <c r="D10">
+        <v>3.8438189256221036</v>
+      </c>
+      <c r="E10">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>385638</v>
+      </c>
+      <c r="C11">
+        <v>10181</v>
+      </c>
+      <c r="D11">
+        <v>2.6400406598934754</v>
+      </c>
+      <c r="E11">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>431682</v>
+      </c>
+      <c r="C12">
+        <v>7142</v>
+      </c>
+      <c r="D12">
+        <v>1.6544586061035669</v>
+      </c>
+      <c r="E12">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>356489</v>
+      </c>
+      <c r="C13">
+        <v>5315</v>
+      </c>
+      <c r="D13">
+        <v>1.4909295939005129</v>
+      </c>
+      <c r="E13">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>408078</v>
+      </c>
+      <c r="C14">
+        <v>4335</v>
+      </c>
+      <c r="D14">
+        <v>1.0622969138252982</v>
+      </c>
+      <c r="E14">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>342328</v>
+      </c>
+      <c r="C15">
+        <v>3219</v>
+      </c>
+      <c r="D15">
+        <v>0.94032623682550076</v>
+      </c>
+      <c r="E15">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>327980</v>
+      </c>
+      <c r="C16">
+        <v>2956</v>
+      </c>
+      <c r="D16">
+        <v>0.90127446795536315</v>
+      </c>
+      <c r="E16">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>384834</v>
+      </c>
+      <c r="C17">
+        <v>5588</v>
+      </c>
+      <c r="D17">
+        <v>1.452054652135726</v>
+      </c>
+      <c r="E17">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>472823</v>
+      </c>
+      <c r="C18">
+        <v>3919</v>
+      </c>
+      <c r="D18">
+        <v>0.82885138836308725</v>
+      </c>
+      <c r="E18">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>512969</v>
+      </c>
+      <c r="C19">
+        <v>3204</v>
+      </c>
+      <c r="D19">
+        <v>0.62459914731689448</v>
+      </c>
+      <c r="E19">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>513572</v>
+      </c>
+      <c r="C20">
+        <v>3042</v>
+      </c>
+      <c r="D20">
+        <v>0.59232201132460494</v>
+      </c>
+      <c r="E20">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <v>544219</v>
+      </c>
+      <c r="C21">
+        <v>3608</v>
+      </c>
+      <c r="D21">
+        <v>0.66296840058873363</v>
+      </c>
+      <c r="E21">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22">
+        <v>556634</v>
+      </c>
+      <c r="C22">
+        <v>4537</v>
+      </c>
+      <c r="D22">
+        <v>0.81507777103087486</v>
+      </c>
+      <c r="E22">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23">
+        <v>589201</v>
+      </c>
+      <c r="C23">
+        <v>5888</v>
+      </c>
+      <c r="D23">
+        <v>0.99931941731259788</v>
+      </c>
+      <c r="E23">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24">
+        <v>719476</v>
+      </c>
+      <c r="C24">
+        <v>7374</v>
+      </c>
+      <c r="D24">
+        <v>1.0249125752631083</v>
+      </c>
+      <c r="E24">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25">
+        <v>871191</v>
+      </c>
+      <c r="C25">
+        <v>8545</v>
+      </c>
+      <c r="D25">
+        <v>0.98084117030593754</v>
+      </c>
+      <c r="E25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <v>1034449</v>
+      </c>
+      <c r="C26">
+        <v>8868</v>
+      </c>
+      <c r="D26">
+        <v>0.85726797551160094</v>
+      </c>
+      <c r="E26">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27">
+        <v>1133623</v>
+      </c>
+      <c r="C27">
+        <v>8273</v>
+      </c>
+      <c r="D27">
+        <v>0.72978406401422702</v>
+      </c>
+      <c r="E27">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28">
+        <v>1052942</v>
+      </c>
+      <c r="C28">
+        <v>8203</v>
+      </c>
+      <c r="D28">
+        <v>0.77905525660482722</v>
+      </c>
+      <c r="E28">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29">
+        <v>1148465</v>
+      </c>
+      <c r="C29">
+        <v>10403</v>
+      </c>
+      <c r="D29">
+        <v>0.90581776545214709</v>
+      </c>
+      <c r="E29">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30">
+        <v>1147879</v>
+      </c>
+      <c r="C30">
+        <v>13647</v>
+      </c>
+      <c r="D30">
+        <v>1.1888883758654005</v>
+      </c>
+      <c r="E30">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31">
+        <v>1220279</v>
+      </c>
+      <c r="C31">
+        <v>15178</v>
+      </c>
+      <c r="D31">
+        <v>1.2438139146867233</v>
+      </c>
+      <c r="E31">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32">
+        <v>1129127</v>
+      </c>
+      <c r="C32">
+        <v>19930</v>
+      </c>
+      <c r="D32">
+        <v>1.7650804559628812</v>
+      </c>
+      <c r="E32">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33">
+        <v>1218988</v>
+      </c>
+      <c r="C33">
+        <v>30220</v>
+      </c>
+      <c r="D33">
+        <v>2.4791056187591676</v>
+      </c>
+      <c r="E33">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34">
+        <v>1284349</v>
+      </c>
+      <c r="C34">
+        <v>46000</v>
+      </c>
+      <c r="D34">
+        <v>3.581581018866367</v>
+      </c>
+      <c r="E34">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35">
+        <v>1445463</v>
+      </c>
+      <c r="C35">
+        <v>80097</v>
+      </c>
+      <c r="D35">
+        <v>5.5412694755936336</v>
+      </c>
+      <c r="E35">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36">
+        <v>1663992</v>
+      </c>
+      <c r="C36">
+        <v>118111</v>
+      </c>
+      <c r="D36">
+        <v>7.0980509521680393</v>
+      </c>
+      <c r="E36">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37">
+        <v>1634729</v>
+      </c>
+      <c r="C37">
+        <v>128537</v>
+      </c>
+      <c r="D37">
+        <v>7.8628934826506418</v>
+      </c>
+      <c r="E37">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38">
+        <v>1467454</v>
+      </c>
+      <c r="C38">
+        <v>128986</v>
+      </c>
+      <c r="D38">
+        <v>8.789781485484383</v>
+      </c>
+      <c r="E38">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39">
+        <v>1400145</v>
+      </c>
+      <c r="C39">
+        <v>131185</v>
+      </c>
+      <c r="D39">
+        <v>9.3693867420874266</v>
+      </c>
+      <c r="E39">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40">
+        <v>1381117</v>
+      </c>
+      <c r="C40">
+        <v>128882</v>
+      </c>
+      <c r="D40">
+        <v>9.3317220771303226</v>
+      </c>
+      <c r="E40">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41">
+        <v>1395790</v>
+      </c>
+      <c r="C41">
+        <v>138305</v>
+      </c>
+      <c r="D41">
+        <v>9.9087255246133008</v>
+      </c>
+      <c r="E41">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42">
+        <v>1516038</v>
+      </c>
+      <c r="C42">
+        <v>169520</v>
+      </c>
+      <c r="D42">
+        <v>11.181777765464981</v>
+      </c>
+      <c r="E42">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43">
+        <v>1672033</v>
+      </c>
+      <c r="C43">
+        <v>188283</v>
+      </c>
+      <c r="D43">
+        <v>11.260722724970142</v>
+      </c>
+      <c r="E43">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44">
+        <v>1090372</v>
+      </c>
+      <c r="C44">
+        <v>141413</v>
+      </c>
+      <c r="D44">
+        <v>12.969243524228427</v>
+      </c>
+      <c r="E44">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45">
+        <v>845729</v>
+      </c>
+      <c r="C45">
+        <v>129930</v>
+      </c>
+      <c r="D45">
+        <v>15.363077297810529</v>
+      </c>
+      <c r="E45">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46">
+        <v>1231405</v>
+      </c>
+      <c r="C46">
+        <v>157772</v>
+      </c>
+      <c r="D46">
+        <v>12.812356617035011</v>
+      </c>
+      <c r="E46">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47">
+        <v>1187564</v>
+      </c>
+      <c r="C47">
+        <v>124037</v>
+      </c>
+      <c r="D47">
+        <v>10.44465814052969</v>
+      </c>
+      <c r="E47">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48">
+        <v>1113690</v>
+      </c>
+      <c r="C48">
+        <v>110163</v>
+      </c>
+      <c r="D48">
+        <v>9.8917113379845372</v>
+      </c>
+      <c r="E48">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49">
+        <v>1151633</v>
+      </c>
+      <c r="C49">
+        <v>97383</v>
+      </c>
+      <c r="D49">
+        <v>8.456079323881827</v>
+      </c>
+      <c r="E49">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>54</v>
+      </c>
+      <c r="B50">
+        <v>1101499</v>
+      </c>
+      <c r="C50">
+        <v>82436</v>
+      </c>
+      <c r="D50">
+        <v>7.4839831901799272</v>
+      </c>
+      <c r="E50">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51">
+        <v>1060602</v>
+      </c>
+      <c r="C51">
+        <v>67882</v>
+      </c>
+      <c r="D51">
+        <v>6.4003273612533258</v>
+      </c>
+      <c r="E51">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52">
+        <v>1103231</v>
+      </c>
+      <c r="C52">
+        <v>67379</v>
+      </c>
+      <c r="D52">
+        <v>6.1074244650485703</v>
+      </c>
+      <c r="E52">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53">
+        <v>1171798</v>
+      </c>
+      <c r="C53">
+        <v>72059</v>
+      </c>
+      <c r="D53">
+        <v>6.149438725787209</v>
+      </c>
+      <c r="E53">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54">
+        <v>1153270</v>
+      </c>
+      <c r="C54">
+        <v>71715</v>
+      </c>
+      <c r="D54">
+        <v>6.218405056925091</v>
+      </c>
+      <c r="E54">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55">
+        <v>1280050</v>
+      </c>
+      <c r="C55">
+        <v>85655</v>
+      </c>
+      <c r="D55">
+        <v>6.6915354868950434</v>
+      </c>
+      <c r="E55">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56">
+        <v>1370314</v>
+      </c>
+      <c r="C56">
+        <v>108108</v>
+      </c>
+      <c r="D56">
+        <v>7.8892866890362363</v>
+      </c>
+      <c r="E56">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>61</v>
+      </c>
+      <c r="B57">
+        <v>1418621</v>
+      </c>
+      <c r="C57">
+        <v>132195</v>
+      </c>
+      <c r="D57">
+        <v>9.3185565418811649</v>
+      </c>
+      <c r="E57">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58">
+        <v>1182767</v>
+      </c>
+      <c r="C58">
+        <v>129217</v>
+      </c>
+      <c r="D58">
+        <v>10.924975079622614</v>
+      </c>
+      <c r="E58">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>63</v>
+      </c>
+      <c r="B59">
+        <v>1174136</v>
+      </c>
+      <c r="C59">
+        <v>141356</v>
+      </c>
+      <c r="D59">
+        <v>12.039150490232817</v>
+      </c>
+      <c r="E59">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>64</v>
+      </c>
+      <c r="B60">
+        <v>1316811</v>
+      </c>
+      <c r="C60">
+        <v>163793</v>
+      </c>
+      <c r="D60">
+        <v>12.438611159839946</v>
+      </c>
+      <c r="E60">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B61">
+        <v>1431964</v>
+      </c>
+      <c r="C61">
+        <v>177643</v>
+      </c>
+      <c r="D61">
+        <v>12.405549301518754</v>
+      </c>
+      <c r="E61">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62">
+        <v>1365624</v>
+      </c>
+      <c r="C62">
+        <v>152430</v>
+      </c>
+      <c r="D62">
+        <v>11.161930370292263</v>
+      </c>
+      <c r="E62">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63">
+        <v>1259852</v>
+      </c>
+      <c r="C63">
+        <v>129035</v>
+      </c>
+      <c r="D63">
+        <v>10.242076053377698</v>
+      </c>
+      <c r="E63">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>68</v>
+      </c>
+      <c r="B64">
+        <v>1103708</v>
+      </c>
+      <c r="C64">
+        <v>90555</v>
+      </c>
+      <c r="D64">
+        <v>8.2046157135764179</v>
+      </c>
+      <c r="E64">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>69</v>
+      </c>
+      <c r="B65">
+        <v>1221100</v>
+      </c>
+      <c r="C65">
+        <v>70443</v>
+      </c>
+      <c r="D65">
+        <v>5.7688150028662681</v>
+      </c>
+      <c r="E65">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66">
+        <v>951220</v>
+      </c>
+      <c r="C66">
+        <v>39462</v>
+      </c>
+      <c r="D66">
+        <v>4.1485671032989213</v>
+      </c>
+      <c r="E66">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>71</v>
+      </c>
+      <c r="B67">
+        <v>883832</v>
+      </c>
+      <c r="C67">
+        <v>27561</v>
+      </c>
+      <c r="D67">
+        <v>3.1183528091311472</v>
+      </c>
+      <c r="E67">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>72</v>
+      </c>
+      <c r="B68">
+        <v>835367</v>
+      </c>
+      <c r="C68">
+        <v>19298</v>
+      </c>
+      <c r="D68">
+        <v>2.3101223773503143</v>
+      </c>
+      <c r="E68">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>73</v>
+      </c>
+      <c r="B69">
+        <v>730722</v>
+      </c>
+      <c r="C69">
+        <v>10462</v>
+      </c>
+      <c r="D69">
+        <v>1.4317346405336093</v>
+      </c>
+      <c r="E69">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>74</v>
+      </c>
+      <c r="B70">
+        <v>714477</v>
+      </c>
+      <c r="C70">
+        <v>6927</v>
+      </c>
+      <c r="D70">
+        <v>0.96952036244693662</v>
+      </c>
+      <c r="E70">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>75</v>
+      </c>
+      <c r="B71">
+        <v>726832</v>
+      </c>
+      <c r="C71">
+        <v>5890</v>
+      </c>
+      <c r="D71">
+        <v>0.81036608184559844</v>
+      </c>
+      <c r="E71">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>76</v>
+      </c>
+      <c r="B72">
+        <v>612225</v>
+      </c>
+      <c r="C72">
+        <v>6872</v>
+      </c>
+      <c r="D72">
+        <v>1.122463146718935</v>
+      </c>
+      <c r="E72">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>77</v>
+      </c>
+      <c r="B73">
+        <v>607770</v>
+      </c>
+      <c r="C73">
+        <v>9864</v>
+      </c>
+      <c r="D73">
+        <v>1.6229823782022805</v>
+      </c>
+      <c r="E73">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>78</v>
+      </c>
+      <c r="B74">
+        <v>594342</v>
+      </c>
+      <c r="C74">
+        <v>13804</v>
+      </c>
+      <c r="D74">
+        <v>2.3225684875038279</v>
+      </c>
+      <c r="E74">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>79</v>
+      </c>
+      <c r="B75">
+        <v>583319</v>
+      </c>
+      <c r="C75">
+        <v>17108</v>
+      </c>
+      <c r="D75">
+        <v>2.9328720648564506</v>
+      </c>
+      <c r="E75">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>80</v>
+      </c>
+      <c r="B76">
+        <v>589841</v>
+      </c>
+      <c r="C76">
+        <v>22500</v>
+      </c>
+      <c r="D76">
+        <v>3.8145873209898942</v>
+      </c>
+      <c r="E76">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>81</v>
+      </c>
+      <c r="B77">
+        <v>567948</v>
+      </c>
+      <c r="C77">
+        <v>34255</v>
+      </c>
+      <c r="D77">
+        <v>6.0313620261009806</v>
+      </c>
+      <c r="E77">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>82</v>
+      </c>
+      <c r="B78">
+        <v>690888</v>
+      </c>
+      <c r="C78">
+        <v>53966</v>
+      </c>
+      <c r="D78">
+        <v>7.8111068653674689</v>
+      </c>
+      <c r="E78">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>83</v>
+      </c>
+      <c r="B79">
+        <v>861596</v>
+      </c>
+      <c r="C79">
+        <v>70512</v>
+      </c>
+      <c r="D79">
+        <v>8.1838820050232357</v>
+      </c>
+      <c r="E79">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>84</v>
+      </c>
+      <c r="B80">
+        <v>946737</v>
+      </c>
+      <c r="C80">
+        <v>82091</v>
+      </c>
+      <c r="D80">
+        <v>8.6709402928162724</v>
+      </c>
+      <c r="E80">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>85</v>
+      </c>
+      <c r="B81">
+        <v>1010977</v>
+      </c>
+      <c r="C81">
+        <v>80004</v>
+      </c>
+      <c r="D81">
+        <v>7.9135331466492325</v>
+      </c>
+      <c r="E81">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>86</v>
+      </c>
+      <c r="B82">
+        <v>982150</v>
+      </c>
+      <c r="C82">
+        <v>72640</v>
+      </c>
+      <c r="D82">
+        <v>7.3960189380440866</v>
+      </c>
+      <c r="E82">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>87</v>
+      </c>
+      <c r="B83">
+        <v>961979</v>
+      </c>
+      <c r="C83">
+        <v>61593</v>
+      </c>
+      <c r="D83">
+        <v>6.4027385213190717</v>
+      </c>
+      <c r="E83">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>88</v>
+      </c>
+      <c r="B84">
+        <v>963970</v>
+      </c>
+      <c r="C84">
+        <v>61710</v>
+      </c>
+      <c r="D84">
+        <v>6.4016515036775008</v>
+      </c>
+      <c r="E84">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>89</v>
+      </c>
+      <c r="B85">
+        <v>957725</v>
+      </c>
+      <c r="C85">
+        <v>62171</v>
+      </c>
+      <c r="D85">
+        <v>6.4915294056226998</v>
+      </c>
+      <c r="E85">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>90</v>
+      </c>
+      <c r="B86">
+        <v>857989</v>
+      </c>
+      <c r="C86">
+        <v>69645</v>
+      </c>
+      <c r="D86">
+        <v>8.1172369342730502</v>
+      </c>
+      <c r="E86">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>91</v>
+      </c>
+      <c r="B87">
+        <v>906917</v>
+      </c>
+      <c r="C87">
+        <v>98591</v>
+      </c>
+      <c r="D87">
+        <v>10.87100583625624</v>
+      </c>
+      <c r="E87">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>92</v>
+      </c>
+      <c r="B88">
+        <v>1163552</v>
+      </c>
+      <c r="C88">
+        <v>141219</v>
+      </c>
+      <c r="D88">
+        <v>12.136887736860922</v>
+      </c>
+      <c r="E88">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>93</v>
+      </c>
+      <c r="B89">
+        <v>1183169</v>
+      </c>
+      <c r="C89">
+        <v>188073</v>
+      </c>
+      <c r="D89">
+        <v>15.895700445160413</v>
+      </c>
+      <c r="E89">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>94</v>
+      </c>
+      <c r="B90">
+        <v>1606571</v>
+      </c>
+      <c r="C90">
+        <v>277377</v>
+      </c>
+      <c r="D90">
+        <v>17.265156659743017</v>
+      </c>
+      <c r="E90">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>95</v>
+      </c>
+      <c r="B91">
+        <v>81975529</v>
+      </c>
+      <c r="C91">
+        <v>5677751</v>
+      </c>
+      <c r="D91" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E91" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="7">
+        <v>71380530</v>
+      </c>
+      <c r="C2" s="7">
+        <v>4564728</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1010977</v>
+      </c>
+      <c r="C3" s="7">
+        <v>80004</v>
+      </c>
+      <c r="D3" s="8">
+        <v>7.9135331466492325</v>
+      </c>
+      <c r="E3" s="6">
+        <v>211</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="7">
+        <v>982150</v>
+      </c>
+      <c r="C4" s="7">
+        <v>72640</v>
+      </c>
+      <c r="D4" s="8">
+        <v>7.3960189380440866</v>
+      </c>
+      <c r="E4" s="6">
+        <v>213</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="7">
+        <v>961979</v>
+      </c>
+      <c r="C5" s="7">
+        <v>61593</v>
+      </c>
+      <c r="D5" s="8">
+        <v>6.4027385213190717</v>
+      </c>
+      <c r="E5" s="6">
+        <v>210</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="7">
+        <v>963970</v>
+      </c>
+      <c r="C6" s="7">
+        <v>61710</v>
+      </c>
+      <c r="D6" s="8">
+        <v>6.4016515036775008</v>
+      </c>
+      <c r="E6" s="6">
+        <v>209</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="7">
+        <v>957725</v>
+      </c>
+      <c r="C7" s="7">
+        <v>62171</v>
+      </c>
+      <c r="D7" s="8">
+        <v>6.4915294056226998</v>
+      </c>
+      <c r="E7" s="6">
+        <v>208</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="7">
+        <v>857989</v>
+      </c>
+      <c r="C8" s="7">
+        <v>69645</v>
+      </c>
+      <c r="D8" s="8">
+        <v>8.1172369342730502</v>
+      </c>
+      <c r="E8" s="6">
+        <v>206</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="7">
+        <v>906917</v>
+      </c>
+      <c r="C9" s="7">
+        <v>98591</v>
+      </c>
+      <c r="D9" s="8">
+        <v>10.87100583625624</v>
+      </c>
+      <c r="E9" s="6">
+        <v>203</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="7">
+        <v>1163552</v>
+      </c>
+      <c r="C10" s="7">
+        <v>141219</v>
+      </c>
+      <c r="D10" s="8">
+        <v>12.136887736860922</v>
+      </c>
+      <c r="E10" s="6">
+        <v>211</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="7">
+        <v>1183169</v>
+      </c>
+      <c r="C11" s="7">
+        <v>188073</v>
+      </c>
+      <c r="D11" s="8">
+        <v>15.895700445160413</v>
+      </c>
+      <c r="E11" s="6">
+        <v>205</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="10">
+        <v>1606571</v>
+      </c>
+      <c r="C12" s="10">
+        <v>277377</v>
+      </c>
+      <c r="D12" s="11">
+        <v>17.265156659743017</v>
+      </c>
+      <c r="E12" s="9">
+        <v>200</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="12">
+        <v>81975529</v>
+      </c>
+      <c r="C13" s="12">
+        <v>5677751</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -828,1812 +2696,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>69493</v>
-      </c>
-      <c r="C2">
-        <v>1722</v>
-      </c>
-      <c r="D2" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E2" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>129291</v>
-      </c>
-      <c r="C3">
-        <v>7502</v>
-      </c>
-      <c r="D3">
-        <v>5.8024147079069692</v>
-      </c>
-      <c r="E3">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>374534</v>
-      </c>
-      <c r="C4">
-        <v>25886</v>
-      </c>
-      <c r="D4">
-        <v>6.9115220514025424</v>
-      </c>
-      <c r="E4">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>377599</v>
-      </c>
-      <c r="C5">
-        <v>33139</v>
-      </c>
-      <c r="D5">
-        <v>8.7762414625038723</v>
-      </c>
-      <c r="E5">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>417646</v>
-      </c>
-      <c r="C6">
-        <v>37649</v>
-      </c>
-      <c r="D6">
-        <v>9.0145721496195339</v>
-      </c>
-      <c r="E6">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>383694</v>
-      </c>
-      <c r="C7">
-        <v>30727</v>
-      </c>
-      <c r="D7">
-        <v>8.0082044545914197</v>
-      </c>
-      <c r="E7">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <v>339983</v>
-      </c>
-      <c r="C8">
-        <v>22724</v>
-      </c>
-      <c r="D8">
-        <v>6.6838636049449534</v>
-      </c>
-      <c r="E8">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9">
-        <v>363659</v>
-      </c>
-      <c r="C9">
-        <v>18127</v>
-      </c>
-      <c r="D9">
-        <v>4.984614707734444</v>
-      </c>
-      <c r="E9">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <v>327799</v>
-      </c>
-      <c r="C10">
-        <v>12600</v>
-      </c>
-      <c r="D10">
-        <v>3.8438189256221036</v>
-      </c>
-      <c r="E10">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <v>385638</v>
-      </c>
-      <c r="C11">
-        <v>10181</v>
-      </c>
-      <c r="D11">
-        <v>2.6400406598934754</v>
-      </c>
-      <c r="E11">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12">
-        <v>431682</v>
-      </c>
-      <c r="C12">
-        <v>7142</v>
-      </c>
-      <c r="D12">
-        <v>1.6544586061035669</v>
-      </c>
-      <c r="E12">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13">
-        <v>356489</v>
-      </c>
-      <c r="C13">
-        <v>5315</v>
-      </c>
-      <c r="D13">
-        <v>1.4909295939005129</v>
-      </c>
-      <c r="E13">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14">
-        <v>408078</v>
-      </c>
-      <c r="C14">
-        <v>4335</v>
-      </c>
-      <c r="D14">
-        <v>1.0622969138252982</v>
-      </c>
-      <c r="E14">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15">
-        <v>342328</v>
-      </c>
-      <c r="C15">
-        <v>3219</v>
-      </c>
-      <c r="D15">
-        <v>0.94032623682550076</v>
-      </c>
-      <c r="E15">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16">
-        <v>327980</v>
-      </c>
-      <c r="C16">
-        <v>2956</v>
-      </c>
-      <c r="D16">
-        <v>0.90127446795536315</v>
-      </c>
-      <c r="E16">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17">
-        <v>384834</v>
-      </c>
-      <c r="C17">
-        <v>5588</v>
-      </c>
-      <c r="D17">
-        <v>1.452054652135726</v>
-      </c>
-      <c r="E17">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18">
-        <v>472823</v>
-      </c>
-      <c r="C18">
-        <v>3919</v>
-      </c>
-      <c r="D18">
-        <v>0.82885138836308725</v>
-      </c>
-      <c r="E18">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19">
-        <v>512969</v>
-      </c>
-      <c r="C19">
-        <v>3204</v>
-      </c>
-      <c r="D19">
-        <v>0.62459914731689448</v>
-      </c>
-      <c r="E19">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20">
-        <v>513572</v>
-      </c>
-      <c r="C20">
-        <v>3042</v>
-      </c>
-      <c r="D20">
-        <v>0.59232201132460494</v>
-      </c>
-      <c r="E20">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21">
-        <v>544219</v>
-      </c>
-      <c r="C21">
-        <v>3608</v>
-      </c>
-      <c r="D21">
-        <v>0.66296840058873363</v>
-      </c>
-      <c r="E21">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22">
-        <v>556634</v>
-      </c>
-      <c r="C22">
-        <v>4537</v>
-      </c>
-      <c r="D22">
-        <v>0.81507777103087486</v>
-      </c>
-      <c r="E22">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23">
-        <v>589201</v>
-      </c>
-      <c r="C23">
-        <v>5888</v>
-      </c>
-      <c r="D23">
-        <v>0.99931941731259788</v>
-      </c>
-      <c r="E23">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24">
-        <v>719476</v>
-      </c>
-      <c r="C24">
-        <v>7374</v>
-      </c>
-      <c r="D24">
-        <v>1.0249125752631083</v>
-      </c>
-      <c r="E24">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25">
-        <v>871191</v>
-      </c>
-      <c r="C25">
-        <v>8545</v>
-      </c>
-      <c r="D25">
-        <v>0.98084117030593754</v>
-      </c>
-      <c r="E25">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26">
-        <v>1034449</v>
-      </c>
-      <c r="C26">
-        <v>8868</v>
-      </c>
-      <c r="D26">
-        <v>0.85726797551160094</v>
-      </c>
-      <c r="E26">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27">
-        <v>1133623</v>
-      </c>
-      <c r="C27">
-        <v>8273</v>
-      </c>
-      <c r="D27">
-        <v>0.72978406401422702</v>
-      </c>
-      <c r="E27">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28">
-        <v>1052942</v>
-      </c>
-      <c r="C28">
-        <v>8203</v>
-      </c>
-      <c r="D28">
-        <v>0.77905525660482722</v>
-      </c>
-      <c r="E28">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29">
-        <v>1148465</v>
-      </c>
-      <c r="C29">
-        <v>10403</v>
-      </c>
-      <c r="D29">
-        <v>0.90581776545214709</v>
-      </c>
-      <c r="E29">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30">
-        <v>1147879</v>
-      </c>
-      <c r="C30">
-        <v>13647</v>
-      </c>
-      <c r="D30">
-        <v>1.1888883758654005</v>
-      </c>
-      <c r="E30">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31">
-        <v>1220279</v>
-      </c>
-      <c r="C31">
-        <v>15178</v>
-      </c>
-      <c r="D31">
-        <v>1.2438139146867233</v>
-      </c>
-      <c r="E31">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32">
-        <v>1129127</v>
-      </c>
-      <c r="C32">
-        <v>19930</v>
-      </c>
-      <c r="D32">
-        <v>1.7650804559628812</v>
-      </c>
-      <c r="E32">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33">
-        <v>1218988</v>
-      </c>
-      <c r="C33">
-        <v>30220</v>
-      </c>
-      <c r="D33">
-        <v>2.4791056187591676</v>
-      </c>
-      <c r="E33">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34">
-        <v>1284349</v>
-      </c>
-      <c r="C34">
-        <v>46000</v>
-      </c>
-      <c r="D34">
-        <v>3.581581018866367</v>
-      </c>
-      <c r="E34">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>39</v>
-      </c>
-      <c r="B35">
-        <v>1445463</v>
-      </c>
-      <c r="C35">
-        <v>80097</v>
-      </c>
-      <c r="D35">
-        <v>5.5412694755936336</v>
-      </c>
-      <c r="E35">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36">
-        <v>1663992</v>
-      </c>
-      <c r="C36">
-        <v>118111</v>
-      </c>
-      <c r="D36">
-        <v>7.0980509521680393</v>
-      </c>
-      <c r="E36">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>41</v>
-      </c>
-      <c r="B37">
-        <v>1634729</v>
-      </c>
-      <c r="C37">
-        <v>128537</v>
-      </c>
-      <c r="D37">
-        <v>7.8628934826506418</v>
-      </c>
-      <c r="E37">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>42</v>
-      </c>
-      <c r="B38">
-        <v>1467454</v>
-      </c>
-      <c r="C38">
-        <v>128986</v>
-      </c>
-      <c r="D38">
-        <v>8.789781485484383</v>
-      </c>
-      <c r="E38">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39">
-        <v>1400145</v>
-      </c>
-      <c r="C39">
-        <v>131185</v>
-      </c>
-      <c r="D39">
-        <v>9.3693867420874266</v>
-      </c>
-      <c r="E39">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40">
-        <v>1381117</v>
-      </c>
-      <c r="C40">
-        <v>128882</v>
-      </c>
-      <c r="D40">
-        <v>9.3317220771303226</v>
-      </c>
-      <c r="E40">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41">
-        <v>1395790</v>
-      </c>
-      <c r="C41">
-        <v>138305</v>
-      </c>
-      <c r="D41">
-        <v>9.9087255246133008</v>
-      </c>
-      <c r="E41">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42">
-        <v>1516038</v>
-      </c>
-      <c r="C42">
-        <v>169520</v>
-      </c>
-      <c r="D42">
-        <v>11.181777765464981</v>
-      </c>
-      <c r="E42">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43">
-        <v>1672033</v>
-      </c>
-      <c r="C43">
-        <v>188283</v>
-      </c>
-      <c r="D43">
-        <v>11.260722724970142</v>
-      </c>
-      <c r="E43">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44">
-        <v>1090372</v>
-      </c>
-      <c r="C44">
-        <v>141413</v>
-      </c>
-      <c r="D44">
-        <v>12.969243524228427</v>
-      </c>
-      <c r="E44">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45">
-        <v>845729</v>
-      </c>
-      <c r="C45">
-        <v>129930</v>
-      </c>
-      <c r="D45">
-        <v>15.363077297810529</v>
-      </c>
-      <c r="E45">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46">
-        <v>1231405</v>
-      </c>
-      <c r="C46">
-        <v>157772</v>
-      </c>
-      <c r="D46">
-        <v>12.812356617035011</v>
-      </c>
-      <c r="E46">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>51</v>
-      </c>
-      <c r="B47">
-        <v>1187564</v>
-      </c>
-      <c r="C47">
-        <v>124037</v>
-      </c>
-      <c r="D47">
-        <v>10.44465814052969</v>
-      </c>
-      <c r="E47">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>52</v>
-      </c>
-      <c r="B48">
-        <v>1113690</v>
-      </c>
-      <c r="C48">
-        <v>110163</v>
-      </c>
-      <c r="D48">
-        <v>9.8917113379845372</v>
-      </c>
-      <c r="E48">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>53</v>
-      </c>
-      <c r="B49">
-        <v>1151633</v>
-      </c>
-      <c r="C49">
-        <v>97383</v>
-      </c>
-      <c r="D49">
-        <v>8.456079323881827</v>
-      </c>
-      <c r="E49">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>54</v>
-      </c>
-      <c r="B50">
-        <v>1101499</v>
-      </c>
-      <c r="C50">
-        <v>82436</v>
-      </c>
-      <c r="D50">
-        <v>7.4839831901799272</v>
-      </c>
-      <c r="E50">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>55</v>
-      </c>
-      <c r="B51">
-        <v>1060602</v>
-      </c>
-      <c r="C51">
-        <v>67882</v>
-      </c>
-      <c r="D51">
-        <v>6.4003273612533258</v>
-      </c>
-      <c r="E51">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52">
-        <v>1103231</v>
-      </c>
-      <c r="C52">
-        <v>67379</v>
-      </c>
-      <c r="D52">
-        <v>6.1074244650485703</v>
-      </c>
-      <c r="E52">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>57</v>
-      </c>
-      <c r="B53">
-        <v>1171798</v>
-      </c>
-      <c r="C53">
-        <v>72059</v>
-      </c>
-      <c r="D53">
-        <v>6.149438725787209</v>
-      </c>
-      <c r="E53">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>58</v>
-      </c>
-      <c r="B54">
-        <v>1153270</v>
-      </c>
-      <c r="C54">
-        <v>71715</v>
-      </c>
-      <c r="D54">
-        <v>6.218405056925091</v>
-      </c>
-      <c r="E54">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>59</v>
-      </c>
-      <c r="B55">
-        <v>1280050</v>
-      </c>
-      <c r="C55">
-        <v>85655</v>
-      </c>
-      <c r="D55">
-        <v>6.6915354868950434</v>
-      </c>
-      <c r="E55">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>60</v>
-      </c>
-      <c r="B56">
-        <v>1370314</v>
-      </c>
-      <c r="C56">
-        <v>108108</v>
-      </c>
-      <c r="D56">
-        <v>7.8892866890362363</v>
-      </c>
-      <c r="E56">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>61</v>
-      </c>
-      <c r="B57">
-        <v>1418621</v>
-      </c>
-      <c r="C57">
-        <v>132195</v>
-      </c>
-      <c r="D57">
-        <v>9.3185565418811649</v>
-      </c>
-      <c r="E57">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>62</v>
-      </c>
-      <c r="B58">
-        <v>1182767</v>
-      </c>
-      <c r="C58">
-        <v>129217</v>
-      </c>
-      <c r="D58">
-        <v>10.924975079622614</v>
-      </c>
-      <c r="E58">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>63</v>
-      </c>
-      <c r="B59">
-        <v>1174136</v>
-      </c>
-      <c r="C59">
-        <v>141356</v>
-      </c>
-      <c r="D59">
-        <v>12.039150490232817</v>
-      </c>
-      <c r="E59">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>64</v>
-      </c>
-      <c r="B60">
-        <v>1316811</v>
-      </c>
-      <c r="C60">
-        <v>163793</v>
-      </c>
-      <c r="D60">
-        <v>12.438611159839946</v>
-      </c>
-      <c r="E60">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>65</v>
-      </c>
-      <c r="B61">
-        <v>1431964</v>
-      </c>
-      <c r="C61">
-        <v>177643</v>
-      </c>
-      <c r="D61">
-        <v>12.405549301518754</v>
-      </c>
-      <c r="E61">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>66</v>
-      </c>
-      <c r="B62">
-        <v>1365624</v>
-      </c>
-      <c r="C62">
-        <v>152430</v>
-      </c>
-      <c r="D62">
-        <v>11.161930370292263</v>
-      </c>
-      <c r="E62">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>67</v>
-      </c>
-      <c r="B63">
-        <v>1259852</v>
-      </c>
-      <c r="C63">
-        <v>129035</v>
-      </c>
-      <c r="D63">
-        <v>10.242076053377698</v>
-      </c>
-      <c r="E63">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>68</v>
-      </c>
-      <c r="B64">
-        <v>1103708</v>
-      </c>
-      <c r="C64">
-        <v>90555</v>
-      </c>
-      <c r="D64">
-        <v>8.2046157135764179</v>
-      </c>
-      <c r="E64">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>69</v>
-      </c>
-      <c r="B65">
-        <v>1221100</v>
-      </c>
-      <c r="C65">
-        <v>70443</v>
-      </c>
-      <c r="D65">
-        <v>5.7688150028662681</v>
-      </c>
-      <c r="E65">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>70</v>
-      </c>
-      <c r="B66">
-        <v>951220</v>
-      </c>
-      <c r="C66">
-        <v>39462</v>
-      </c>
-      <c r="D66">
-        <v>4.1485671032989213</v>
-      </c>
-      <c r="E66">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>71</v>
-      </c>
-      <c r="B67">
-        <v>883832</v>
-      </c>
-      <c r="C67">
-        <v>27561</v>
-      </c>
-      <c r="D67">
-        <v>3.1183528091311472</v>
-      </c>
-      <c r="E67">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>72</v>
-      </c>
-      <c r="B68">
-        <v>835367</v>
-      </c>
-      <c r="C68">
-        <v>19298</v>
-      </c>
-      <c r="D68">
-        <v>2.3101223773503143</v>
-      </c>
-      <c r="E68">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>73</v>
-      </c>
-      <c r="B69">
-        <v>730722</v>
-      </c>
-      <c r="C69">
-        <v>10462</v>
-      </c>
-      <c r="D69">
-        <v>1.4317346405336093</v>
-      </c>
-      <c r="E69">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>74</v>
-      </c>
-      <c r="B70">
-        <v>714477</v>
-      </c>
-      <c r="C70">
-        <v>6927</v>
-      </c>
-      <c r="D70">
-        <v>0.96952036244693662</v>
-      </c>
-      <c r="E70">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>75</v>
-      </c>
-      <c r="B71">
-        <v>726832</v>
-      </c>
-      <c r="C71">
-        <v>5890</v>
-      </c>
-      <c r="D71">
-        <v>0.81036608184559844</v>
-      </c>
-      <c r="E71">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>76</v>
-      </c>
-      <c r="B72">
-        <v>612225</v>
-      </c>
-      <c r="C72">
-        <v>6872</v>
-      </c>
-      <c r="D72">
-        <v>1.122463146718935</v>
-      </c>
-      <c r="E72">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>77</v>
-      </c>
-      <c r="B73">
-        <v>607770</v>
-      </c>
-      <c r="C73">
-        <v>9864</v>
-      </c>
-      <c r="D73">
-        <v>1.6229823782022805</v>
-      </c>
-      <c r="E73">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>78</v>
-      </c>
-      <c r="B74">
-        <v>594342</v>
-      </c>
-      <c r="C74">
-        <v>13804</v>
-      </c>
-      <c r="D74">
-        <v>2.3225684875038279</v>
-      </c>
-      <c r="E74">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>79</v>
-      </c>
-      <c r="B75">
-        <v>583319</v>
-      </c>
-      <c r="C75">
-        <v>17108</v>
-      </c>
-      <c r="D75">
-        <v>2.9328720648564506</v>
-      </c>
-      <c r="E75">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>80</v>
-      </c>
-      <c r="B76">
-        <v>589841</v>
-      </c>
-      <c r="C76">
-        <v>22500</v>
-      </c>
-      <c r="D76">
-        <v>3.8145873209898942</v>
-      </c>
-      <c r="E76">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>81</v>
-      </c>
-      <c r="B77">
-        <v>567948</v>
-      </c>
-      <c r="C77">
-        <v>34255</v>
-      </c>
-      <c r="D77">
-        <v>6.0313620261009806</v>
-      </c>
-      <c r="E77">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>82</v>
-      </c>
-      <c r="B78">
-        <v>690888</v>
-      </c>
-      <c r="C78">
-        <v>53966</v>
-      </c>
-      <c r="D78">
-        <v>7.8111068653674689</v>
-      </c>
-      <c r="E78">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>83</v>
-      </c>
-      <c r="B79">
-        <v>861596</v>
-      </c>
-      <c r="C79">
-        <v>70512</v>
-      </c>
-      <c r="D79">
-        <v>8.1838820050232357</v>
-      </c>
-      <c r="E79">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>84</v>
-      </c>
-      <c r="B80">
-        <v>946737</v>
-      </c>
-      <c r="C80">
-        <v>82091</v>
-      </c>
-      <c r="D80">
-        <v>8.6709402928162724</v>
-      </c>
-      <c r="E80">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>85</v>
-      </c>
-      <c r="B81">
-        <v>1010977</v>
-      </c>
-      <c r="C81">
-        <v>80004</v>
-      </c>
-      <c r="D81">
-        <v>7.9135331466492325</v>
-      </c>
-      <c r="E81">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>86</v>
-      </c>
-      <c r="B82">
-        <v>982150</v>
-      </c>
-      <c r="C82">
-        <v>72640</v>
-      </c>
-      <c r="D82">
-        <v>7.3960189380440866</v>
-      </c>
-      <c r="E82">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>87</v>
-      </c>
-      <c r="B83">
-        <v>961979</v>
-      </c>
-      <c r="C83">
-        <v>61593</v>
-      </c>
-      <c r="D83">
-        <v>6.4027385213190717</v>
-      </c>
-      <c r="E83">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>88</v>
-      </c>
-      <c r="B84">
-        <v>963970</v>
-      </c>
-      <c r="C84">
-        <v>61710</v>
-      </c>
-      <c r="D84">
-        <v>6.4016515036775008</v>
-      </c>
-      <c r="E84">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>89</v>
-      </c>
-      <c r="B85">
-        <v>957725</v>
-      </c>
-      <c r="C85">
-        <v>62171</v>
-      </c>
-      <c r="D85">
-        <v>6.4915294056226998</v>
-      </c>
-      <c r="E85">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>90</v>
-      </c>
-      <c r="B86">
-        <v>857989</v>
-      </c>
-      <c r="C86">
-        <v>69645</v>
-      </c>
-      <c r="D86">
-        <v>8.1172369342730502</v>
-      </c>
-      <c r="E86">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>91</v>
-      </c>
-      <c r="B87">
-        <v>906917</v>
-      </c>
-      <c r="C87">
-        <v>98591</v>
-      </c>
-      <c r="D87">
-        <v>10.87100583625624</v>
-      </c>
-      <c r="E87">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>92</v>
-      </c>
-      <c r="B88">
-        <v>1159772</v>
-      </c>
-      <c r="C88">
-        <v>140857</v>
-      </c>
-      <c r="D88">
-        <v>12.145231993874658</v>
-      </c>
-      <c r="E88">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>93</v>
-      </c>
-      <c r="B89">
-        <v>1166712</v>
-      </c>
-      <c r="C89">
-        <v>187018</v>
-      </c>
-      <c r="D89">
-        <v>16.029491425476039</v>
-      </c>
-      <c r="E89">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>94</v>
-      </c>
-      <c r="B90">
-        <v>80348721</v>
-      </c>
-      <c r="C90">
-        <v>5398957</v>
-      </c>
-      <c r="D90" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="E90" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="30.28515625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" s="7">
-        <v>70433793</v>
-      </c>
-      <c r="C2" s="7">
-        <v>4482637</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="7">
-        <v>946737</v>
-      </c>
-      <c r="C3" s="7">
-        <v>82091</v>
-      </c>
-      <c r="D3" s="8">
-        <v>8.6709402928162724</v>
-      </c>
-      <c r="E3" s="6">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" s="7">
-        <v>1010977</v>
-      </c>
-      <c r="C4" s="7">
-        <v>80004</v>
-      </c>
-      <c r="D4" s="8">
-        <v>7.9135331466492325</v>
-      </c>
-      <c r="E4" s="6">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="7">
-        <v>982150</v>
-      </c>
-      <c r="C5" s="7">
-        <v>72640</v>
-      </c>
-      <c r="D5" s="8">
-        <v>7.3960189380440866</v>
-      </c>
-      <c r="E5" s="6">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B6" s="7">
-        <v>961979</v>
-      </c>
-      <c r="C6" s="7">
-        <v>61593</v>
-      </c>
-      <c r="D6" s="8">
-        <v>6.4027385213190717</v>
-      </c>
-      <c r="E6" s="6">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" s="7">
-        <v>963970</v>
-      </c>
-      <c r="C7" s="7">
-        <v>61710</v>
-      </c>
-      <c r="D7" s="8">
-        <v>6.4016515036775008</v>
-      </c>
-      <c r="E7" s="6">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" s="7">
-        <v>957725</v>
-      </c>
-      <c r="C8" s="7">
-        <v>62171</v>
-      </c>
-      <c r="D8" s="8">
-        <v>6.4915294056226998</v>
-      </c>
-      <c r="E8" s="6">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="7">
-        <v>857989</v>
-      </c>
-      <c r="C9" s="7">
-        <v>69645</v>
-      </c>
-      <c r="D9" s="8">
-        <v>8.1172369342730502</v>
-      </c>
-      <c r="E9" s="6">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="7">
-        <v>906917</v>
-      </c>
-      <c r="C10" s="7">
-        <v>98591</v>
-      </c>
-      <c r="D10" s="8">
-        <v>10.87100583625624</v>
-      </c>
-      <c r="E10" s="6">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B11" s="7">
-        <v>1159772</v>
-      </c>
-      <c r="C11" s="7">
-        <v>140857</v>
-      </c>
-      <c r="D11" s="8">
-        <v>12.145231993874658</v>
-      </c>
-      <c r="E11" s="6">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="10">
-        <v>1166712</v>
-      </c>
-      <c r="C12" s="10">
-        <v>187018</v>
-      </c>
-      <c r="D12" s="11">
-        <v>16.029491425476039</v>
-      </c>
-      <c r="E12" s="9">
-        <v>196</v>
-      </c>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B13" s="12">
-        <v>80348721</v>
-      </c>
-      <c r="C13" s="12">
-        <v>5398957</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E89"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2783,7 +2858,7 @@
         <v>151063</v>
       </c>
       <c r="D10">
-        <v>981515</v>
+        <v>981515.00199999998</v>
       </c>
       <c r="E10">
         <v>777476</v>
@@ -2800,7 +2875,7 @@
         <v>156630</v>
       </c>
       <c r="D11">
-        <v>1030122</v>
+        <v>1030122.5</v>
       </c>
       <c r="E11">
         <v>825063</v>
@@ -2817,7 +2892,7 @@
         <v>159588</v>
       </c>
       <c r="D12">
-        <v>1057365</v>
+        <v>1057365.5</v>
       </c>
       <c r="E12">
         <v>837380</v>
@@ -2851,7 +2926,7 @@
         <v>167525</v>
       </c>
       <c r="D14">
-        <v>1115162</v>
+        <v>1115162.5</v>
       </c>
       <c r="E14">
         <v>904760</v>
@@ -2885,7 +2960,7 @@
         <v>169858</v>
       </c>
       <c r="D16">
-        <v>1123147</v>
+        <v>1123147.5</v>
       </c>
       <c r="E16">
         <v>951456</v>
@@ -3344,7 +3419,7 @@
         <v>338390</v>
       </c>
       <c r="D43">
-        <v>1468673</v>
+        <v>1468673.7</v>
       </c>
       <c r="E43">
         <v>1288535</v>
@@ -3361,7 +3436,7 @@
         <v>331055</v>
       </c>
       <c r="D44">
-        <v>1331534</v>
+        <v>1331534.94</v>
       </c>
       <c r="E44">
         <v>1190932</v>
@@ -3480,7 +3555,7 @@
         <v>350601</v>
       </c>
       <c r="D51">
-        <v>2344259</v>
+        <v>2344259.7142857141</v>
       </c>
       <c r="E51">
         <v>2219267</v>
@@ -3684,7 +3759,7 @@
         <v>366449</v>
       </c>
       <c r="D63">
-        <v>2456944</v>
+        <v>2456944.5</v>
       </c>
       <c r="E63">
         <v>2369910</v>
@@ -4103,33 +4178,50 @@
         <v>93</v>
       </c>
       <c r="B88">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C88">
-        <v>341602</v>
+        <v>342952</v>
       </c>
       <c r="D88">
-        <v>2291202</v>
+        <v>2298652</v>
       </c>
       <c r="E88">
-        <v>2217944</v>
+        <v>2220394</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B89">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="C89">
-        <v>344176</v>
+        <v>347326</v>
       </c>
       <c r="D89">
-        <v>2299500</v>
+        <v>2318950</v>
       </c>
       <c r="E89">
-        <v>2242842</v>
+        <v>2255792</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>102</v>
+      </c>
+      <c r="B90">
+        <v>177</v>
+      </c>
+      <c r="C90">
+        <v>347789</v>
+      </c>
+      <c r="D90">
+        <v>2330153</v>
+      </c>
+      <c r="E90">
+        <v>2272613</v>
       </c>
     </row>
   </sheetData>
@@ -4147,223 +4239,223 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B2">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C2">
-        <v>348487</v>
+        <v>362613</v>
       </c>
       <c r="D2">
-        <v>2327587</v>
+        <v>2435855</v>
       </c>
       <c r="E2">
-        <v>2258159</v>
+        <v>2355657</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B3">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C3">
-        <v>362613</v>
+        <v>363137</v>
       </c>
       <c r="D3">
-        <v>2435855</v>
+        <v>2437937</v>
       </c>
       <c r="E3">
-        <v>2355657</v>
+        <v>2349449</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B4">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C4">
-        <v>363137</v>
+        <v>365781</v>
       </c>
       <c r="D4">
-        <v>2437937</v>
+        <v>2445235</v>
       </c>
       <c r="E4">
-        <v>2349449</v>
+        <v>2368947</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B5">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C5">
-        <v>365781</v>
+        <v>367591</v>
       </c>
       <c r="D5">
-        <v>2445235</v>
+        <v>2472697</v>
       </c>
       <c r="E5">
-        <v>2368947</v>
+        <v>2394889</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B6">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C6">
-        <v>367591</v>
+        <v>366991</v>
       </c>
       <c r="D6">
-        <v>2472697</v>
+        <v>2465545</v>
       </c>
       <c r="E6">
-        <v>2394889</v>
+        <v>2247987</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B7">
         <v>186</v>
       </c>
       <c r="C7">
-        <v>366991</v>
+        <v>365311</v>
       </c>
       <c r="D7">
-        <v>2465545</v>
+        <v>2454295</v>
       </c>
       <c r="E7">
-        <v>2247987</v>
+        <v>2245127</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B8">
         <v>186</v>
       </c>
       <c r="C8">
-        <v>365311</v>
+        <v>344259</v>
       </c>
       <c r="D8">
-        <v>2454295</v>
+        <v>2295241</v>
       </c>
       <c r="E8">
-        <v>2245127</v>
+        <v>2223153</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B9">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C9">
-        <v>344259</v>
+        <v>341422</v>
       </c>
       <c r="D9">
-        <v>2295241</v>
+        <v>2282832</v>
       </c>
       <c r="E9">
-        <v>2223153</v>
+        <v>2208464</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B10">
         <v>181</v>
       </c>
       <c r="C10">
-        <v>341422</v>
+        <v>341992</v>
       </c>
       <c r="D10">
-        <v>2282832</v>
+        <v>2289882</v>
       </c>
       <c r="E10">
-        <v>2208464</v>
+        <v>2205614</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B11">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C11">
-        <v>341992</v>
+        <v>342952</v>
       </c>
       <c r="D11">
-        <v>2289882</v>
+        <v>2298652</v>
       </c>
       <c r="E11">
-        <v>2205614</v>
+        <v>2220394</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B12">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C12">
-        <v>341602</v>
+        <v>347326</v>
       </c>
       <c r="D12">
-        <v>2291202</v>
+        <v>2318950</v>
       </c>
       <c r="E12">
-        <v>2217944</v>
+        <v>2255792</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B13">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C13">
-        <v>344176</v>
+        <v>347789</v>
       </c>
       <c r="D13">
-        <v>2299500</v>
+        <v>2330153</v>
       </c>
       <c r="E13">
-        <v>2242842</v>
+        <v>2272613</v>
       </c>
     </row>
   </sheetData>
@@ -4373,7 +4465,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4381,13 +4473,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5300,6 +5392,17 @@
         <v>44</v>
       </c>
       <c r="C84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>0</v>
+      </c>
+      <c r="B85">
+        <v>45</v>
+      </c>
+      <c r="C85">
         <v>0</v>
       </c>
     </row>

</xml_diff>